<commit_message>
Extract out Postal Codes into Excel/JSON for more accurate Geocoding
</commit_message>
<xml_diff>
--- a/toilet data/sgtoilets-address-only.xlsx
+++ b/toilet data/sgtoilets-address-only.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\OneDrive\Desktop\TF\tf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\OneDrive\Desktop\TF\tf\toilet data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD37B93-C73C-4865-A728-8D48FC72FB08}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE46F4A0-3723-41F9-A930-69CB5D555ABD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{71E80B8A-1A49-4CC9-90C5-1870DC05784B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{71E80B8A-1A49-4CC9-90C5-1870DC05784B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -821,9 +821,6 @@
     <t>475 Choa Chu Kang Avenue 3  S(680475)</t>
   </si>
   <si>
-    <t>Blk 399 Yung Sheng Road (Near Party World/NTUC)</t>
-  </si>
-  <si>
     <t>624 Choa Chu Kang Street 62  S(680624)</t>
   </si>
   <si>
@@ -831,6 +828,9 @@
   </si>
   <si>
     <t>to be deleted</t>
+  </si>
+  <si>
+    <t>Blk 399 Yung Sheng Road (Near Party World/NTUC)(610399)</t>
   </si>
 </sst>
 </file>
@@ -1185,28 +1185,31 @@
   <dimension ref="A1:B274"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="20.453125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1214,7 +1217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1222,7 +1225,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1230,7 +1233,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1238,7 +1241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1246,7 +1249,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1254,7 +1257,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1262,7 +1265,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1270,7 +1273,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1278,7 +1281,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1286,7 +1289,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1294,7 +1297,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1302,7 +1305,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1310,7 +1313,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1318,7 +1321,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1326,7 +1329,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1334,7 +1337,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1342,7 +1345,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1350,7 +1353,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1358,7 +1361,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1366,7 +1369,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1374,7 +1377,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1382,7 +1385,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1390,7 +1393,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1398,7 +1401,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1406,7 +1409,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1414,7 +1417,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1422,7 +1425,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1430,7 +1433,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1438,7 +1441,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1446,7 +1449,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1454,7 +1457,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1462,7 +1465,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1470,7 +1473,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1478,7 +1481,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1486,7 +1489,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1494,7 +1497,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1502,7 +1505,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1510,7 +1513,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1518,7 +1521,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1526,7 +1529,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1534,7 +1537,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1542,7 +1545,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1550,7 +1553,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1558,7 +1561,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1566,7 +1569,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1574,7 +1577,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>47</v>
       </c>
@@ -1582,7 +1585,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>48</v>
       </c>
@@ -1590,7 +1593,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>49</v>
       </c>
@@ -1598,7 +1601,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>50</v>
       </c>
@@ -1606,7 +1609,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>51</v>
       </c>
@@ -1614,7 +1617,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>52</v>
       </c>
@@ -1622,7 +1625,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>53</v>
       </c>
@@ -1630,7 +1633,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>54</v>
       </c>
@@ -1638,7 +1641,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>55</v>
       </c>
@@ -1646,7 +1649,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>56</v>
       </c>
@@ -1654,7 +1657,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>57</v>
       </c>
@@ -1662,7 +1665,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>58</v>
       </c>
@@ -1670,7 +1673,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>59</v>
       </c>
@@ -1678,7 +1681,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>60</v>
       </c>
@@ -1686,7 +1689,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>61</v>
       </c>
@@ -1694,7 +1697,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>62</v>
       </c>
@@ -1702,7 +1705,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>63</v>
       </c>
@@ -1710,7 +1713,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>64</v>
       </c>
@@ -1718,7 +1721,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>65</v>
       </c>
@@ -1726,7 +1729,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>66</v>
       </c>
@@ -1734,7 +1737,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>67</v>
       </c>
@@ -1742,7 +1745,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>68</v>
       </c>
@@ -1750,7 +1753,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>69</v>
       </c>
@@ -1758,7 +1761,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>70</v>
       </c>
@@ -1766,7 +1769,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>71</v>
       </c>
@@ -1774,7 +1777,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>72</v>
       </c>
@@ -1782,7 +1785,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>73</v>
       </c>
@@ -1790,7 +1793,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>74</v>
       </c>
@@ -1798,7 +1801,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>75</v>
       </c>
@@ -1806,7 +1809,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>76</v>
       </c>
@@ -1814,7 +1817,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>77</v>
       </c>
@@ -1822,7 +1825,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>78</v>
       </c>
@@ -1830,7 +1833,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>79</v>
       </c>
@@ -1838,7 +1841,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>80</v>
       </c>
@@ -1846,7 +1849,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>81</v>
       </c>
@@ -1854,7 +1857,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>82</v>
       </c>
@@ -1862,7 +1865,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>83</v>
       </c>
@@ -1870,7 +1873,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>84</v>
       </c>
@@ -1878,7 +1881,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>85</v>
       </c>
@@ -1886,7 +1889,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>86</v>
       </c>
@@ -1894,7 +1897,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>87</v>
       </c>
@@ -1902,7 +1905,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>88</v>
       </c>
@@ -1910,7 +1913,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>89</v>
       </c>
@@ -1918,7 +1921,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>90</v>
       </c>
@@ -1926,7 +1929,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>91</v>
       </c>
@@ -1934,7 +1937,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>92</v>
       </c>
@@ -1942,7 +1945,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>93</v>
       </c>
@@ -1950,7 +1953,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>94</v>
       </c>
@@ -1958,7 +1961,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>95</v>
       </c>
@@ -1966,7 +1969,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>96</v>
       </c>
@@ -1974,7 +1977,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>97</v>
       </c>
@@ -1982,7 +1985,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>98</v>
       </c>
@@ -1990,7 +1993,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>99</v>
       </c>
@@ -1998,7 +2001,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>100</v>
       </c>
@@ -2006,7 +2009,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>101</v>
       </c>
@@ -2014,7 +2017,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>102</v>
       </c>
@@ -2022,7 +2025,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>103</v>
       </c>
@@ -2030,7 +2033,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>104</v>
       </c>
@@ -2038,7 +2041,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>105</v>
       </c>
@@ -2046,7 +2049,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>106</v>
       </c>
@@ -2054,7 +2057,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>107</v>
       </c>
@@ -2062,7 +2065,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>108</v>
       </c>
@@ -2070,7 +2073,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>109</v>
       </c>
@@ -2078,7 +2081,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>110</v>
       </c>
@@ -2086,7 +2089,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>111</v>
       </c>
@@ -2094,7 +2097,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>112</v>
       </c>
@@ -2102,7 +2105,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>113</v>
       </c>
@@ -2110,7 +2113,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>114</v>
       </c>
@@ -2118,7 +2121,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>115</v>
       </c>
@@ -2126,7 +2129,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>116</v>
       </c>
@@ -2134,7 +2137,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>117</v>
       </c>
@@ -2142,7 +2145,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>118</v>
       </c>
@@ -2150,7 +2153,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>119</v>
       </c>
@@ -2158,7 +2161,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>120</v>
       </c>
@@ -2166,7 +2169,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>121</v>
       </c>
@@ -2174,7 +2177,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>122</v>
       </c>
@@ -2182,7 +2185,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>123</v>
       </c>
@@ -2190,7 +2193,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>124</v>
       </c>
@@ -2198,7 +2201,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>125</v>
       </c>
@@ -2206,7 +2209,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>126</v>
       </c>
@@ -2214,7 +2217,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>127</v>
       </c>
@@ -2222,7 +2225,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>128</v>
       </c>
@@ -2230,7 +2233,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>129</v>
       </c>
@@ -2238,7 +2241,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>130</v>
       </c>
@@ -2246,7 +2249,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>131</v>
       </c>
@@ -2254,7 +2257,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>132</v>
       </c>
@@ -2262,7 +2265,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>133</v>
       </c>
@@ -2270,7 +2273,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>134</v>
       </c>
@@ -2278,7 +2281,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>135</v>
       </c>
@@ -2286,7 +2289,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>136</v>
       </c>
@@ -2294,7 +2297,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>137</v>
       </c>
@@ -2302,7 +2305,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>138</v>
       </c>
@@ -2310,7 +2313,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>139</v>
       </c>
@@ -2318,7 +2321,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>140</v>
       </c>
@@ -2326,7 +2329,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>141</v>
       </c>
@@ -2334,7 +2337,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>142</v>
       </c>
@@ -2342,7 +2345,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>143</v>
       </c>
@@ -2350,7 +2353,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>144</v>
       </c>
@@ -2358,7 +2361,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>145</v>
       </c>
@@ -2366,7 +2369,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>146</v>
       </c>
@@ -2374,7 +2377,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>147</v>
       </c>
@@ -2382,7 +2385,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>148</v>
       </c>
@@ -2390,7 +2393,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>149</v>
       </c>
@@ -2398,7 +2401,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>150</v>
       </c>
@@ -2406,7 +2409,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>151</v>
       </c>
@@ -2414,7 +2417,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>152</v>
       </c>
@@ -2422,7 +2425,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>153</v>
       </c>
@@ -2430,7 +2433,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>154</v>
       </c>
@@ -2438,7 +2441,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>155</v>
       </c>
@@ -2446,7 +2449,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>156</v>
       </c>
@@ -2454,7 +2457,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>157</v>
       </c>
@@ -2462,7 +2465,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>158</v>
       </c>
@@ -2470,7 +2473,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>159</v>
       </c>
@@ -2478,7 +2481,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>160</v>
       </c>
@@ -2486,7 +2489,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>161</v>
       </c>
@@ -2494,7 +2497,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>162</v>
       </c>
@@ -2502,7 +2505,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>163</v>
       </c>
@@ -2510,7 +2513,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>164</v>
       </c>
@@ -2518,7 +2521,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>165</v>
       </c>
@@ -2526,7 +2529,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>166</v>
       </c>
@@ -2534,7 +2537,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>167</v>
       </c>
@@ -2542,7 +2545,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>168</v>
       </c>
@@ -2550,7 +2553,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>169</v>
       </c>
@@ -2558,7 +2561,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>170</v>
       </c>
@@ -2566,7 +2569,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>171</v>
       </c>
@@ -2574,7 +2577,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>172</v>
       </c>
@@ -2582,7 +2585,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>173</v>
       </c>
@@ -2590,7 +2593,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>174</v>
       </c>
@@ -2598,7 +2601,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>175</v>
       </c>
@@ -2606,7 +2609,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>176</v>
       </c>
@@ -2614,7 +2617,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179">
         <v>177</v>
       </c>
@@ -2622,7 +2625,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>178</v>
       </c>
@@ -2630,7 +2633,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>179</v>
       </c>
@@ -2638,7 +2641,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182">
         <v>180</v>
       </c>
@@ -2646,7 +2649,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183">
         <v>181</v>
       </c>
@@ -2654,7 +2657,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184">
         <v>182</v>
       </c>
@@ -2662,7 +2665,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>183</v>
       </c>
@@ -2670,7 +2673,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186">
         <v>184</v>
       </c>
@@ -2678,7 +2681,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187">
         <v>185</v>
       </c>
@@ -2686,7 +2689,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188">
         <v>186</v>
       </c>
@@ -2694,7 +2697,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>187</v>
       </c>
@@ -2702,7 +2705,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190">
         <v>188</v>
       </c>
@@ -2710,7 +2713,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191">
         <v>189</v>
       </c>
@@ -2718,7 +2721,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192">
         <v>190</v>
       </c>
@@ -2726,7 +2729,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>191</v>
       </c>
@@ -2734,7 +2737,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194">
         <v>192</v>
       </c>
@@ -2742,7 +2745,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195">
         <v>193</v>
       </c>
@@ -2750,7 +2753,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196">
         <v>194</v>
       </c>
@@ -2758,7 +2761,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197">
         <v>195</v>
       </c>
@@ -2766,7 +2769,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198">
         <v>196</v>
       </c>
@@ -2774,7 +2777,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199">
         <v>197</v>
       </c>
@@ -2782,7 +2785,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200">
         <v>198</v>
       </c>
@@ -2790,7 +2793,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201">
         <v>199</v>
       </c>
@@ -2798,7 +2801,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202">
         <v>200</v>
       </c>
@@ -2806,7 +2809,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203">
         <v>201</v>
       </c>
@@ -2814,7 +2817,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204">
         <v>202</v>
       </c>
@@ -2822,7 +2825,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205">
         <v>203</v>
       </c>
@@ -2830,7 +2833,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206">
         <v>204</v>
       </c>
@@ -2838,7 +2841,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207">
         <v>205</v>
       </c>
@@ -2846,7 +2849,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208">
         <v>206</v>
       </c>
@@ -2854,7 +2857,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209">
         <v>207</v>
       </c>
@@ -2862,7 +2865,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210">
         <v>208</v>
       </c>
@@ -2870,7 +2873,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211">
         <v>209</v>
       </c>
@@ -2878,7 +2881,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212">
         <v>210</v>
       </c>
@@ -2886,7 +2889,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213">
         <v>211</v>
       </c>
@@ -2894,7 +2897,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214">
         <v>212</v>
       </c>
@@ -2902,7 +2905,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215">
         <v>213</v>
       </c>
@@ -2910,7 +2913,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216">
         <v>214</v>
       </c>
@@ -2918,7 +2921,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217">
         <v>215</v>
       </c>
@@ -2926,7 +2929,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A218">
         <v>216</v>
       </c>
@@ -2934,7 +2937,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219">
         <v>217</v>
       </c>
@@ -2942,7 +2945,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220">
         <v>218</v>
       </c>
@@ -2950,7 +2953,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221">
         <v>219</v>
       </c>
@@ -2958,7 +2961,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A222">
         <v>220</v>
       </c>
@@ -2966,7 +2969,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223">
         <v>221</v>
       </c>
@@ -2974,7 +2977,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224">
         <v>222</v>
       </c>
@@ -2982,7 +2985,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225">
         <v>223</v>
       </c>
@@ -2990,7 +2993,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226">
         <v>224</v>
       </c>
@@ -2998,7 +3001,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227">
         <v>225</v>
       </c>
@@ -3006,7 +3009,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228">
         <v>226</v>
       </c>
@@ -3014,7 +3017,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229">
         <v>227</v>
       </c>
@@ -3022,7 +3025,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230">
         <v>228</v>
       </c>
@@ -3030,7 +3033,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231">
         <v>229</v>
       </c>
@@ -3038,7 +3041,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232">
         <v>230</v>
       </c>
@@ -3046,7 +3049,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233">
         <v>231</v>
       </c>
@@ -3054,7 +3057,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234">
         <v>232</v>
       </c>
@@ -3062,7 +3065,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235">
         <v>233</v>
       </c>
@@ -3070,7 +3073,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236">
         <v>234</v>
       </c>
@@ -3078,7 +3081,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237">
         <v>235</v>
       </c>
@@ -3086,7 +3089,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238">
         <v>236</v>
       </c>
@@ -3094,7 +3097,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239">
         <v>237</v>
       </c>
@@ -3102,7 +3105,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240">
         <v>238</v>
       </c>
@@ -3110,7 +3113,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241">
         <v>239</v>
       </c>
@@ -3118,7 +3121,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242">
         <v>240</v>
       </c>
@@ -3126,7 +3129,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243">
         <v>241</v>
       </c>
@@ -3134,7 +3137,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244">
         <v>242</v>
       </c>
@@ -3142,7 +3145,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245">
         <v>243</v>
       </c>
@@ -3150,7 +3153,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246">
         <v>244</v>
       </c>
@@ -3158,7 +3161,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247">
         <v>245</v>
       </c>
@@ -3166,7 +3169,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248">
         <v>246</v>
       </c>
@@ -3174,7 +3177,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A249">
         <v>247</v>
       </c>
@@ -3182,7 +3185,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A250">
         <v>248</v>
       </c>
@@ -3190,7 +3193,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A251">
         <v>249</v>
       </c>
@@ -3198,7 +3201,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252">
         <v>250</v>
       </c>
@@ -3206,7 +3209,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A253">
         <v>251</v>
       </c>
@@ -3214,7 +3217,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A254">
         <v>252</v>
       </c>
@@ -3222,7 +3225,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A255">
         <v>253</v>
       </c>
@@ -3230,7 +3233,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A256">
         <v>254</v>
       </c>
@@ -3238,7 +3241,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A257">
         <v>255</v>
       </c>
@@ -3246,7 +3249,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A258">
         <v>256</v>
       </c>
@@ -3254,7 +3257,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A259">
         <v>257</v>
       </c>
@@ -3262,7 +3265,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A260">
         <v>258</v>
       </c>
@@ -3270,7 +3273,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A261">
         <v>259</v>
       </c>
@@ -3278,7 +3281,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A262">
         <v>260</v>
       </c>
@@ -3286,7 +3289,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A263">
         <v>261</v>
       </c>
@@ -3294,7 +3297,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A264">
         <v>262</v>
       </c>
@@ -3302,7 +3305,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A265">
         <v>263</v>
       </c>
@@ -3310,7 +3313,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A266">
         <v>264</v>
       </c>
@@ -3318,7 +3321,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A267">
         <v>265</v>
       </c>
@@ -3326,7 +3329,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A268">
         <v>266</v>
       </c>
@@ -3334,7 +3337,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A269">
         <v>267</v>
       </c>
@@ -3342,7 +3345,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A270">
         <v>268</v>
       </c>
@@ -3350,7 +3353,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A271">
         <v>269</v>
       </c>
@@ -3358,7 +3361,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A272">
         <v>270</v>
       </c>
@@ -3366,20 +3369,20 @@
         <v>262</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A273">
         <v>271</v>
       </c>
       <c r="B273" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A274">
         <v>272</v>
       </c>
       <c r="B274" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>